<commit_message>
Redoing the entire run as the excel was dodgy
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tasika-my.sharepoint.com/personal/ben_couser_tasika_co_uk/Documents/Documents/UiPath/theBanks_scrapping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{29D66757-F905-40E8-83FA-DB2FB4C7D936}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{755E1275-077A-43E1-AFA3-DC2D8932CA0D}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{29D66757-F905-40E8-83FA-DB2FB4C7D936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{322FF19C-8828-4136-8098-BA9C6B772BF1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{EC6DB724-433F-4BB9-927B-70EBABB7ACFF}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11835" xr2:uid="{EC6DB724-433F-4BB9-927B-70EBABB7ACFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,7 @@
     <t>12471.90 mln GBP</t>
   </si>
   <si>
-    <t>+44 08000664429</t>
+    <t>50 St Mary Axe, KT17 1BS, London, United Kingdom</t>
   </si>
 </sst>
 </file>

</xml_diff>